<commit_message>
add orderstatus controller, service, logic, repo; fix update product logic
</commit_message>
<xml_diff>
--- a/src/main/resources/products.xlsx
+++ b/src/main/resources/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Java\MyProject1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956463FF-DF0C-4648-B3D2-EB6BFB19ADCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD02225-A15E-40A6-8EA4-125C72F338F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DCF39F51-7C80-405A-9E9D-9F0F360744FB}"/>
   </bookViews>
@@ -103,10 +103,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,12 +423,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.796875" style="1"/>
   </cols>
   <sheetData>
@@ -440,7 +439,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -449,12 +448,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>10000</v>
       </c>
       <c r="D2" t="s">
@@ -463,12 +462,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>10000</v>
       </c>
       <c r="D3" t="s">
@@ -477,12 +476,12 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>1000000</v>
       </c>
       <c r="D4" t="s">
@@ -491,12 +490,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>10900.5</v>
       </c>
       <c r="D5" t="s">
@@ -505,12 +504,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>10000.02</v>
       </c>
       <c r="D6" t="s">

</xml_diff>